<commit_message>
before jeff touched it
</commit_message>
<xml_diff>
--- a/FPRS FP Key.xlsx
+++ b/FPRS FP Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnwilsoniv/Documents/open2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E347254F-CEDC-8341-8986-532CE001F77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70CD013-B5DA-944E-8A0E-DB6DAA7B6947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{E0432988-A6B7-6546-8BAE-33B1504704C1}"/>
+    <workbookView xWindow="10240" yWindow="1820" windowWidth="28800" windowHeight="16340" xr2:uid="{E0432988-A6B7-6546-8BAE-33B1504704C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="68">
   <si>
     <t>Patient</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>IMG_0579</t>
+  </si>
+  <si>
+    <t>IMG_0592</t>
+  </si>
+  <si>
+    <t>IMG_0861</t>
+  </si>
+  <si>
+    <t>IMG_0942</t>
   </si>
 </sst>
 </file>
@@ -610,13 +619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615D0A9E-AF70-D448-94AF-BE95A416A179}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1323,57 +1332,57 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" t="s">
-        <v>13</v>
-      </c>
-      <c r="M18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -1397,27 +1406,27 @@
         <v>13</v>
       </c>
       <c r="L19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
@@ -1429,7 +1438,7 @@
         <v>13</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
         <v>13</v>
@@ -1438,156 +1447,156 @@
         <v>13</v>
       </c>
       <c r="L20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>16</v>
@@ -1610,7 +1619,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
@@ -1625,7 +1634,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>15</v>
@@ -1651,9 +1660,9 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1663,13 +1672,13 @@
         <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>13</v>
@@ -1678,13 +1687,13 @@
         <v>13</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>13</v>
@@ -1692,7 +1701,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
@@ -1719,7 +1728,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>13</v>
@@ -1728,12 +1737,12 @@
         <v>13</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
@@ -1745,10 +1754,10 @@
         <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>15</v>
@@ -1774,7 +1783,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
@@ -1789,7 +1798,7 @@
         <v>15</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>15</v>
@@ -1815,48 +1824,48 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" t="s">
-        <v>13</v>
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -1871,7 +1880,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>15</v>
@@ -1897,25 +1906,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>13</v>
@@ -1924,13 +1933,13 @@
         <v>13</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>13</v>
@@ -1938,51 +1947,51 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>13</v>
@@ -1991,16 +2000,16 @@
         <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>13</v>
@@ -2020,25 +2029,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>13</v>
@@ -2047,13 +2056,13 @@
         <v>13</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>13</v>
@@ -2061,40 +2070,40 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>13</v>
@@ -2102,28 +2111,28 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>13</v>
@@ -2135,97 +2144,97 @@
         <v>13</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" t="s">
-        <v>13</v>
-      </c>
-      <c r="L38" t="s">
-        <v>13</v>
-      </c>
-      <c r="M38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" t="s">
-        <v>13</v>
-      </c>
-      <c r="L39" t="s">
-        <v>13</v>
-      </c>
-      <c r="M39" t="s">
-        <v>16</v>
+        <v>50</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>15</v>
@@ -2266,107 +2275,107 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" t="s">
+        <v>13</v>
+      </c>
+      <c r="M41" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>13</v>
@@ -2378,121 +2387,121 @@
         <v>13</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" t="s">
-        <v>13</v>
-      </c>
-      <c r="L44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" t="s">
-        <v>13</v>
-      </c>
-      <c r="L45" t="s">
-        <v>13</v>
-      </c>
-      <c r="M45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>13</v>
@@ -2501,10 +2510,10 @@
         <v>13</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>13</v>
@@ -2512,124 +2521,247 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L47" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" t="s">
+        <v>13</v>
+      </c>
+      <c r="L48" t="s">
+        <v>13</v>
+      </c>
+      <c r="M48" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M49" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M52" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>